<commit_message>
Code cleanup and comments
</commit_message>
<xml_diff>
--- a/misc/actions.xlsx
+++ b/misc/actions.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dropbox\proj_x\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\digger\misc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{B05745F5-8681-43B9-8EBF-E793F9D443B1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{424D1827-A05F-4052-AFF1-25299B95221F}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3410" yWindow="0" windowWidth="30990" windowHeight="11120" xr2:uid="{802663B2-CC43-438C-84AF-C0C1A5C6E7DB}"/>
+    <workbookView xWindow="6820" yWindow="0" windowWidth="25180" windowHeight="11120" xr2:uid="{802663B2-CC43-438C-84AF-C0C1A5C6E7DB}"/>
   </bookViews>
   <sheets>
     <sheet name="List1" sheetId="1" r:id="rId1"/>
@@ -39,16 +39,16 @@
     <t>special ability</t>
   </si>
   <si>
-    <t>location 1…location nm</t>
-  </si>
-  <si>
-    <t>target 1…target na</t>
-  </si>
-  <si>
-    <t>target 1…target nr</t>
-  </si>
-  <si>
-    <t>ability 1…ability ns (but can be targeted, so more cases possible)</t>
+    <t>target 1…target N</t>
+  </si>
+  <si>
+    <t>target 1…target M</t>
+  </si>
+  <si>
+    <t>location 1…location L</t>
+  </si>
+  <si>
+    <t>ability 1…ability S (but can be targeted, so more cases possible)</t>
   </si>
 </sst>
 </file>
@@ -404,13 +404,13 @@
   <dimension ref="A2:B5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="16.54296875" customWidth="1"/>
-    <col min="2" max="2" width="22.08984375" customWidth="1"/>
+    <col min="2" max="2" width="24.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
@@ -418,7 +418,7 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>6</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
@@ -434,7 +434,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">

</xml_diff>